<commit_message>
hard coding of age/grade equiv lookup relationships
</commit_message>
<xml_diff>
--- a/INPUT-FILES/OES-INPUT-TABLES/TOD-S/TODS-age-equiv.xlsx
+++ b/INPUT-FILES/OES-INPUT-TABLES/TOD-S/TODS-age-equiv.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Library/CloudStorage/OneDrive-WesternPsychologicalServices/Desktop/R/TOD-R/INPUT-FILES/OES-INPUT-TABLES/TOD-S/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA731B00-4AC3-EA41-93A1-C307690C4A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C84AFB-B73B-B140-BDBC-5A0DF8C48FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EABC92A2-809A-4DFA-ACE4-11ABAF20006A}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{EABC92A2-809A-4DFA-ACE4-11ABAF20006A}"/>
   </bookViews>
   <sheets>
     <sheet name="age" sheetId="1" r:id="rId1"/>
+    <sheet name="PV" sheetId="2" r:id="rId2"/>
+    <sheet name="LWC" sheetId="3" r:id="rId3"/>
+    <sheet name="WRF" sheetId="4" r:id="rId4"/>
+    <sheet name="QRF" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="127">
   <si>
     <t>&lt; Start age</t>
   </si>
@@ -309,15 +313,130 @@
   </si>
   <si>
     <t>QRF raw</t>
+  </si>
+  <si>
+    <t>"&lt; Start age",</t>
+  </si>
+  <si>
+    <t>"5:0 to 5:3",</t>
+  </si>
+  <si>
+    <t>"5:4 to 5:7",</t>
+  </si>
+  <si>
+    <t>"5:8 to 5:11",</t>
+  </si>
+  <si>
+    <t>"6:0 to 6:3",</t>
+  </si>
+  <si>
+    <t>"6:4 to 6:7",</t>
+  </si>
+  <si>
+    <t>"6:8 to 6:11",</t>
+  </si>
+  <si>
+    <t>"7:0 to 7:3",</t>
+  </si>
+  <si>
+    <t>"7:4 to 7:7",</t>
+  </si>
+  <si>
+    <t>"7:8 to 7:11",</t>
+  </si>
+  <si>
+    <t>"8:0 to 8:5",</t>
+  </si>
+  <si>
+    <t>"8:6 to 8:11",</t>
+  </si>
+  <si>
+    <t>"9:0 to 9:5",</t>
+  </si>
+  <si>
+    <t>"9:6 to 9:11",</t>
+  </si>
+  <si>
+    <t>"10:0 to 10:5",</t>
+  </si>
+  <si>
+    <t>"10:6 to 10:11",</t>
+  </si>
+  <si>
+    <t>"11:0 to 11:5",</t>
+  </si>
+  <si>
+    <t>"11:6 to 11:11",</t>
+  </si>
+  <si>
+    <t>"12:0 to 12:5",</t>
+  </si>
+  <si>
+    <t>"12:6 to 12:11",</t>
+  </si>
+  <si>
+    <t>"13:0 to 13:11",</t>
+  </si>
+  <si>
+    <t>"14:0 to 14:11",</t>
+  </si>
+  <si>
+    <t>"15:0 to 16:11",</t>
+  </si>
+  <si>
+    <t>"17:0 to 18:11",</t>
+  </si>
+  <si>
+    <t>"&gt;stop age",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">) ~ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &amp; between(raw, </t>
+  </si>
+  <si>
+    <t>"PV"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp; test == </t>
+  </si>
+  <si>
+    <t xml:space="preserve">norm_group == </t>
+  </si>
+  <si>
+    <t>"age"</t>
+  </si>
+  <si>
+    <t>"LWC"</t>
+  </si>
+  <si>
+    <t>"WRF"</t>
+  </si>
+  <si>
+    <t>"QRF"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp; between(raw, </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -337,12 +456,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -357,15 +482,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -682,10 +813,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8247680A-F953-459F-B5BA-666871AD1791}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1145,6 +1279,2822 @@
       <c r="A29" s="1"/>
     </row>
   </sheetData>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0263B0BE-7FCC-194F-BAC4-A396D50D6491}">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection sqref="A1:J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1">
+        <v>96</v>
+      </c>
+      <c r="I1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2">
+        <v>97</v>
+      </c>
+      <c r="G2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2">
+        <v>101</v>
+      </c>
+      <c r="I2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3">
+        <v>102</v>
+      </c>
+      <c r="G3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3">
+        <v>103</v>
+      </c>
+      <c r="I3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4">
+        <v>104</v>
+      </c>
+      <c r="G4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4">
+        <v>105</v>
+      </c>
+      <c r="I4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5">
+        <v>106</v>
+      </c>
+      <c r="G5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5">
+        <v>107</v>
+      </c>
+      <c r="I5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6">
+        <v>108</v>
+      </c>
+      <c r="G6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6">
+        <v>109</v>
+      </c>
+      <c r="I6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7">
+        <v>110</v>
+      </c>
+      <c r="G7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7">
+        <v>111</v>
+      </c>
+      <c r="I7" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8">
+        <v>112</v>
+      </c>
+      <c r="G8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8">
+        <v>113</v>
+      </c>
+      <c r="I8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9">
+        <v>114</v>
+      </c>
+      <c r="G9" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9">
+        <v>115</v>
+      </c>
+      <c r="I9" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10">
+        <v>116</v>
+      </c>
+      <c r="G10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10">
+        <v>116</v>
+      </c>
+      <c r="I10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" s="3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11">
+        <v>117</v>
+      </c>
+      <c r="G11" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11">
+        <v>118</v>
+      </c>
+      <c r="I11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12">
+        <v>119</v>
+      </c>
+      <c r="G12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12">
+        <v>120</v>
+      </c>
+      <c r="I12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13">
+        <v>121</v>
+      </c>
+      <c r="G13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13">
+        <v>122</v>
+      </c>
+      <c r="I13" t="s">
+        <v>116</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14">
+        <v>123</v>
+      </c>
+      <c r="G14" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14">
+        <v>123</v>
+      </c>
+      <c r="I14" t="s">
+        <v>116</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="L14" s="3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F15">
+        <v>124</v>
+      </c>
+      <c r="G15" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15">
+        <v>125</v>
+      </c>
+      <c r="I15" t="s">
+        <v>116</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F16">
+        <v>126</v>
+      </c>
+      <c r="G16" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16">
+        <v>126</v>
+      </c>
+      <c r="I16" t="s">
+        <v>116</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="L16" s="3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17">
+        <v>127</v>
+      </c>
+      <c r="G17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17">
+        <v>127</v>
+      </c>
+      <c r="I17" t="s">
+        <v>116</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="L17" s="3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" t="s">
+        <v>119</v>
+      </c>
+      <c r="E18" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18">
+        <v>128</v>
+      </c>
+      <c r="G18" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18">
+        <v>128</v>
+      </c>
+      <c r="I18" t="s">
+        <v>116</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="L18" s="3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" t="s">
+        <v>119</v>
+      </c>
+      <c r="E19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19">
+        <v>129</v>
+      </c>
+      <c r="G19" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19">
+        <v>129</v>
+      </c>
+      <c r="I19" t="s">
+        <v>116</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="L19" s="3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20">
+        <v>130</v>
+      </c>
+      <c r="G20" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20">
+        <v>130</v>
+      </c>
+      <c r="I20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="L20" s="3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21">
+        <v>131</v>
+      </c>
+      <c r="G21" t="s">
+        <v>117</v>
+      </c>
+      <c r="H21">
+        <v>131</v>
+      </c>
+      <c r="I21" t="s">
+        <v>116</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="L21" s="3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22">
+        <v>132</v>
+      </c>
+      <c r="G22" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22">
+        <v>132</v>
+      </c>
+      <c r="I22" t="s">
+        <v>116</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="L22" s="3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23">
+        <v>133</v>
+      </c>
+      <c r="G23" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23">
+        <v>135</v>
+      </c>
+      <c r="I23" t="s">
+        <v>116</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24">
+        <v>136</v>
+      </c>
+      <c r="G24" t="s">
+        <v>117</v>
+      </c>
+      <c r="H24">
+        <v>138</v>
+      </c>
+      <c r="I24" t="s">
+        <v>116</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25">
+        <v>139</v>
+      </c>
+      <c r="G25" t="s">
+        <v>117</v>
+      </c>
+      <c r="H25">
+        <v>173</v>
+      </c>
+      <c r="I25" t="s">
+        <v>116</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7D5003-64B5-D047-AFD1-7C8EB5156E9A}">
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection sqref="A1:J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1">
+        <v>82</v>
+      </c>
+      <c r="I1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2">
+        <v>83</v>
+      </c>
+      <c r="G2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2">
+        <v>88</v>
+      </c>
+      <c r="I2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3">
+        <v>89</v>
+      </c>
+      <c r="G3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3">
+        <v>91</v>
+      </c>
+      <c r="I3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4">
+        <v>92</v>
+      </c>
+      <c r="G4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4">
+        <v>95</v>
+      </c>
+      <c r="I4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5">
+        <v>96</v>
+      </c>
+      <c r="G5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5">
+        <v>98</v>
+      </c>
+      <c r="I5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6">
+        <v>99</v>
+      </c>
+      <c r="G6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6">
+        <v>102</v>
+      </c>
+      <c r="I6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7">
+        <v>103</v>
+      </c>
+      <c r="G7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7">
+        <v>105</v>
+      </c>
+      <c r="I7" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8">
+        <v>106</v>
+      </c>
+      <c r="G8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8">
+        <v>107</v>
+      </c>
+      <c r="I8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9">
+        <v>108</v>
+      </c>
+      <c r="G9" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9">
+        <v>110</v>
+      </c>
+      <c r="I9" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10">
+        <v>111</v>
+      </c>
+      <c r="G10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10">
+        <v>112</v>
+      </c>
+      <c r="I10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11">
+        <v>113</v>
+      </c>
+      <c r="G11" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11">
+        <v>115</v>
+      </c>
+      <c r="I11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12">
+        <v>116</v>
+      </c>
+      <c r="G12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12">
+        <v>118</v>
+      </c>
+      <c r="I12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13">
+        <v>119</v>
+      </c>
+      <c r="G13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13">
+        <v>120</v>
+      </c>
+      <c r="I13" t="s">
+        <v>116</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14">
+        <v>121</v>
+      </c>
+      <c r="G14" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14">
+        <v>122</v>
+      </c>
+      <c r="I14" t="s">
+        <v>116</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F15">
+        <v>123</v>
+      </c>
+      <c r="G15" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15">
+        <v>124</v>
+      </c>
+      <c r="I15" t="s">
+        <v>116</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" t="s">
+        <v>123</v>
+      </c>
+      <c r="E16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F16">
+        <v>125</v>
+      </c>
+      <c r="G16" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16">
+        <v>125</v>
+      </c>
+      <c r="I16" t="s">
+        <v>116</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="L16" s="3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17">
+        <v>126</v>
+      </c>
+      <c r="G17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17">
+        <v>126</v>
+      </c>
+      <c r="I17" t="s">
+        <v>116</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="L17" s="3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18">
+        <v>127</v>
+      </c>
+      <c r="G18" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18">
+        <v>127</v>
+      </c>
+      <c r="I18" t="s">
+        <v>116</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="L18" s="3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19">
+        <v>128</v>
+      </c>
+      <c r="G19" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19">
+        <v>129</v>
+      </c>
+      <c r="I19" t="s">
+        <v>116</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" t="s">
+        <v>123</v>
+      </c>
+      <c r="E20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20">
+        <v>130</v>
+      </c>
+      <c r="G20" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20">
+        <v>131</v>
+      </c>
+      <c r="I20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21">
+        <v>132</v>
+      </c>
+      <c r="G21" t="s">
+        <v>117</v>
+      </c>
+      <c r="H21">
+        <v>134</v>
+      </c>
+      <c r="I21" t="s">
+        <v>116</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22">
+        <v>135</v>
+      </c>
+      <c r="G22" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22">
+        <v>139</v>
+      </c>
+      <c r="I22" t="s">
+        <v>116</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23">
+        <v>140</v>
+      </c>
+      <c r="G23" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23">
+        <v>168</v>
+      </c>
+      <c r="I23" t="s">
+        <v>116</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF06DE10-BAFD-EA47-84D1-5D86674FEE6F}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection sqref="A1:J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10">
+        <v>31</v>
+      </c>
+      <c r="I10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11">
+        <v>68</v>
+      </c>
+      <c r="I11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E01A5D1-D85D-8B4F-85C3-D0D87169F52D}">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection sqref="A1:J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L3" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7">
+        <v>33</v>
+      </c>
+      <c r="I7" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8">
+        <v>34</v>
+      </c>
+      <c r="G8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F9">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9">
+        <v>37</v>
+      </c>
+      <c r="I9" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10">
+        <v>38</v>
+      </c>
+      <c r="G10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10">
+        <v>39</v>
+      </c>
+      <c r="I10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F11">
+        <v>40</v>
+      </c>
+      <c r="G11" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11">
+        <v>41</v>
+      </c>
+      <c r="I11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12">
+        <v>43</v>
+      </c>
+      <c r="I12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" t="s">
+        <v>126</v>
+      </c>
+      <c r="F13">
+        <v>44</v>
+      </c>
+      <c r="G13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13">
+        <v>44</v>
+      </c>
+      <c r="I13" t="s">
+        <v>116</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="L13" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14">
+        <v>45</v>
+      </c>
+      <c r="G14" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14">
+        <v>46</v>
+      </c>
+      <c r="I14" t="s">
+        <v>116</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F15">
+        <v>47</v>
+      </c>
+      <c r="G15" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15">
+        <v>48</v>
+      </c>
+      <c r="I15" t="s">
+        <v>116</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16">
+        <v>49</v>
+      </c>
+      <c r="G16" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16">
+        <v>51</v>
+      </c>
+      <c r="I16" t="s">
+        <v>116</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" t="s">
+        <v>126</v>
+      </c>
+      <c r="F17">
+        <v>52</v>
+      </c>
+      <c r="G17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17">
+        <v>54</v>
+      </c>
+      <c r="I17" t="s">
+        <v>116</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18">
+        <v>55</v>
+      </c>
+      <c r="G18" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18">
+        <v>61</v>
+      </c>
+      <c r="I18" t="s">
+        <v>116</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" t="s">
+        <v>126</v>
+      </c>
+      <c r="F19">
+        <v>62</v>
+      </c>
+      <c r="G19" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19">
+        <v>93</v>
+      </c>
+      <c r="I19" t="s">
+        <v>116</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>